<commit_message>
dane saki + dane psy
</commit_message>
<xml_diff>
--- a/UniwersytetDzieci/SSaki/ssaki.xlsx
+++ b/UniwersytetDzieci/SSaki/ssaki.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17220" tabRatio="500"/>
@@ -66,6 +66,12 @@
     <t>Polska nazwa</t>
   </si>
   <si>
+    <t>Kapibara wielka</t>
+  </si>
+  <si>
+    <t>Niedźwiedź polarny</t>
+  </si>
+  <si>
     <t>Świnionos malutki</t>
   </si>
   <si>
@@ -81,22 +87,17 @@
     <t>Wombat tasmański</t>
   </si>
   <si>
-    <t>Kapibara wielka</t>
-  </si>
-  <si>
     <t>Człowiek</t>
   </si>
   <si>
-    <t>Niedźwiedź polarny</t>
-  </si>
-  <si>
     <t>Żyrafa</t>
   </si>
   <si>
     <t>Słoń afrykański</t>
   </si>
   <si>
-    <t>Płetwal błękitny</t>
+    <t>Płetwal
+blekitny</t>
   </si>
 </sst>
 </file>
@@ -170,10 +171,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -524,7 +528,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -535,7 +539,7 @@
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -549,12 +553,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -563,12 +567,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1">
         <v>18</v>
@@ -577,12 +581,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1">
         <v>40</v>
@@ -591,12 +595,12 @@
         <v>350</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1">
         <v>100</v>
@@ -605,12 +609,12 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1">
         <v>120</v>
@@ -619,12 +623,12 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
         <v>134</v>
@@ -633,12 +637,12 @@
         <v>66000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1">
         <v>174</v>
@@ -647,12 +651,12 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1">
         <v>260</v>
@@ -661,7 +665,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -675,7 +679,7 @@
         <v>1900000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="1" customFormat="1">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -689,11 +693,11 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1">
+    <row r="12" spans="1:4" ht="30">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="1">

</xml_diff>